<commit_message>
Updated Visualize, started on adding matches to schedule and refactored the bulky inline script of index.html to index.js
</commit_message>
<xml_diff>
--- a/match_history.xlsx
+++ b/match_history.xlsx
@@ -346,7 +346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ1"/>
+  <dimension ref="A1:AN2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -382,157 +382,363 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>entry.Match.preloaded_balls</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>entry.Match.auto_route</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>entry.Match.baseline</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>entry.Match.upper_auto</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>entry.Match.lower_auto</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>entry.Match.fouls_auto</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>entry.Match.missed_balls_auto</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>entry.Match.auto_fouls</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
         <is>
           <t>entry.Match.auto_comment</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>entry.Match.upper</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>entry.Match.lower</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>entry.Match.balls_collected</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>entry.Match.missed_balls</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>entry.Match.ball_intake_type</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>entry.Match.intake_type</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
         <is>
           <t>entry.Match.under_defense</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>entry.Match.fouls</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>entry.Match.played_defense</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>entry.Match.defense_timer</t>
-        </is>
-      </c>
       <c r="T1" t="inlineStr">
         <is>
+          <t>entry.Match.defended_by</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>entry.Match.offensive_fouls</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>entry.Match.defense_time</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
           <t>entry.Match.defense_rating</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>entry.Match.defense_fouls</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>entry.Match.team_defended</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>entry.Match.able_to_push</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>entry.Match.lock_status</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
         <is>
           <t>entry.Match.endgame_action</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>entry.Match.climb_timer</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>entry.Match.climbed</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>entry.Match.climb_time</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
         <is>
           <t>entry.Match.climb_attempts</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>entry.Match.climb_comments</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>entry.Match.hp_fouls</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>entry.Match.dt_fouls</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>entry.Match.fouls_hp</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>entry.Match.fouls_driver</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
         <is>
           <t>entry.Match.yellow_card</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>entry.Match.disabled</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>entry.Match.yellow_card_description</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>entry.Match.scouter_name</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>entry.Match.comment</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>entry.Match.created_at</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>entry.Match.team_ownership</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>610</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>2022-01-29 16:19:16.124033</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>4343</t>
         </is>
       </c>
     </row>
@@ -547,7 +753,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:BQ4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -675,115 +881,309 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>610</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>West Coast Drive</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Nitrile</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Falcon 500</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>neat</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>alexander</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
           <t>4343</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+    </row>
+    <row r="3">
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>610</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>West Coast Drive</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Nitrile</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>Falcon 500</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>neat</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AS3" t="inlineStr">
+        <is>
+          <t>alexander</t>
+        </is>
+      </c>
+      <c r="AT3" t="inlineStr">
+        <is>
+          <t>4343</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="AU4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AV4" t="inlineStr">
+        <is>
+          <t>914</t>
+        </is>
+      </c>
+      <c r="AW4" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="AX4" t="inlineStr">
+        <is>
+          <t>Kitbot</t>
+        </is>
+      </c>
+      <c r="AY4" t="inlineStr">
+        <is>
+          <t>Andymark White Hi-Grip</t>
+        </is>
+      </c>
+      <c r="AZ4" t="inlineStr">
+        <is>
+          <t>Neo</t>
+        </is>
+      </c>
+      <c r="BA4" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="BB4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BC4" t="inlineStr"/>
+      <c r="BD4" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="BE4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pickup extra and shoot both </t>
+        </is>
+      </c>
+      <c r="BF4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BG4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BH4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BI4" t="inlineStr">
+        <is>
+          <t>Vectored cut bumper</t>
+        </is>
+      </c>
+      <c r="BJ4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BK4" t="inlineStr">
+        <is>
+          <t>Hooded flywheel</t>
+        </is>
+      </c>
+      <c r="BL4" t="inlineStr">
         <is>
           <t>False</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
+      <c r="BM4" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="BN4" t="inlineStr"/>
+      <c r="BO4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BP4" t="inlineStr">
+        <is>
+          <t>NickKerstens</t>
+        </is>
+      </c>
+      <c r="BQ4" t="inlineStr">
         <is>
           <t>4343</t>
         </is>

</xml_diff>